<commit_message>
MOD: Se actulizan las condiciones para la entrega del ejercicio en clase
</commit_message>
<xml_diff>
--- a/material/Tecnicas/Ejercicios/Clase24-Marzo2020/GruposTrabajo.xlsx
+++ b/material/Tecnicas/Ejercicios/Clase24-Marzo2020/GruposTrabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\GIT\lfrincon\material\Tecnicas\Ejercicios\Clase24-Marzo2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3B0295B-F709-4052-BA50-96ED72F2FCBA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799B82E4-8E34-4776-A293-46842C40576B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEFF666A-288D-42FA-BD65-FB453038D7DB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Trabajo grupal</t>
   </si>
@@ -135,10 +135,40 @@
     <t>G6</t>
   </si>
   <si>
-    <t>G7</t>
-  </si>
-  <si>
     <t>Grupo</t>
+  </si>
+  <si>
+    <t>esta viajando a cali</t>
+  </si>
+  <si>
+    <t>no me contesto</t>
+  </si>
+  <si>
+    <t>hable con el pendiente seguimiento</t>
+  </si>
+  <si>
+    <t>hable co el</t>
+  </si>
+  <si>
+    <t>Va a trabajar junto con juan jose fernandez</t>
+  </si>
+  <si>
+    <t>esta enferma</t>
+  </si>
+  <si>
+    <t>seguimiento</t>
+  </si>
+  <si>
+    <t>Pendiente revisar el código</t>
+  </si>
+  <si>
+    <t>ya hablé con ella</t>
+  </si>
+  <si>
+    <t>Pendiente ver el código</t>
+  </si>
+  <si>
+    <t>Faltó</t>
   </si>
 </sst>
 </file>
@@ -207,7 +237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,29 +607,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E81D04-F79C-4865-8FE2-D656BBB027A1}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="6.21875" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -609,8 +640,11 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -620,8 +654,11 @@
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -631,8 +668,11 @@
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -642,8 +682,11 @@
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -653,8 +696,11 @@
       <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -664,8 +710,11 @@
       <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
@@ -675,8 +724,11 @@
       <c r="D8" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -686,8 +738,11 @@
       <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
@@ -697,8 +752,11 @@
       <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -708,21 +766,27 @@
       <c r="D11" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
@@ -730,21 +794,22 @@
       <c r="D13" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
+      <c r="E14" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>